<commit_message>
add back in equal-workers
</commit_message>
<xml_diff>
--- a/simple-hashTimes.xlsx
+++ b/simple-hashTimes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/johnpeterson/Documents/UTexas CS/PS/cs380p-f23/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D88EDE7-DFFE-9747-82F5-8FEAED718608}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92EF5EBF-223E-3846-A57A-DA101FB11450}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2380" yWindow="3500" windowWidth="26580" windowHeight="17440" activeTab="2" xr2:uid="{09B1B139-03D2-1C4D-B9A6-5AC75A022D8A}"/>
+    <workbookView xWindow="2380" yWindow="3500" windowWidth="26580" windowHeight="17440" xr2:uid="{09B1B139-03D2-1C4D-B9A6-5AC75A022D8A}"/>
   </bookViews>
   <sheets>
     <sheet name="hashTime" sheetId="1" r:id="rId1"/>
@@ -18,27 +18,27 @@
     <sheet name="compareTreeTime" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">hashTime!$B$31:$B$60</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">hashTime!$C$30</definedName>
-    <definedName name="_xlchart.v1.10" hidden="1">hashTime!$B$31:$B$60</definedName>
-    <definedName name="_xlchart.v1.11" hidden="1">hashTime!$C$30</definedName>
-    <definedName name="_xlchart.v1.12" hidden="1">hashTime!$C$31:$C$60</definedName>
-    <definedName name="_xlchart.v1.13" hidden="1">hashTime!$D$30</definedName>
-    <definedName name="_xlchart.v1.14" hidden="1">hashTime!$D$31:$D$60</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">hashTime!$C$31:$C$60</definedName>
+    <definedName name="_xlchart.v1.0" hidden="1">hashTime!$B$32:$B$61</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">hashTime!$C$31</definedName>
+    <definedName name="_xlchart.v1.10" hidden="1">hashTime!$B$32:$B$61</definedName>
+    <definedName name="_xlchart.v1.11" hidden="1">hashTime!$C$31</definedName>
+    <definedName name="_xlchart.v1.12" hidden="1">hashTime!$C$32:$C$61</definedName>
+    <definedName name="_xlchart.v1.13" hidden="1">hashTime!$D$31</definedName>
+    <definedName name="_xlchart.v1.14" hidden="1">hashTime!$D$32:$D$61</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">hashTime!$C$32:$C$61</definedName>
     <definedName name="_xlchart.v1.21" hidden="1">compareTreeTime!$B$1</definedName>
     <definedName name="_xlchart.v1.22" hidden="1">compareTreeTime!$B$2:$B$10</definedName>
     <definedName name="_xlchart.v1.23" hidden="1">compareTreeTime!$C$1</definedName>
     <definedName name="_xlchart.v1.24" hidden="1">compareTreeTime!$C$2:$C$10</definedName>
     <definedName name="_xlchart.v1.25" hidden="1">compareTreeTime!$D$1</definedName>
     <definedName name="_xlchart.v1.26" hidden="1">compareTreeTime!$D$2:$D$10</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">hashTime!$D$30</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">hashTime!$D$31:$D$60</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">hashTime!$B$31:$B$60</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">hashTime!$C$30</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">hashTime!$C$31:$C$60</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">hashTime!$D$30</definedName>
-    <definedName name="_xlchart.v1.9" hidden="1">hashTime!$D$31:$D$60</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">hashTime!$D$31</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">hashTime!$D$32:$D$61</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">hashTime!$B$32:$B$61</definedName>
+    <definedName name="_xlchart.v1.6" hidden="1">hashTime!$C$31</definedName>
+    <definedName name="_xlchart.v1.7" hidden="1">hashTime!$C$32:$C$61</definedName>
+    <definedName name="_xlchart.v1.8" hidden="1">hashTime!$D$31</definedName>
+    <definedName name="_xlchart.v1.9" hidden="1">hashTime!$D$32:$D$61</definedName>
     <definedName name="_xlchart.v2.15" hidden="1">compareTreeTime!$B$1</definedName>
     <definedName name="_xlchart.v2.16" hidden="1">compareTreeTime!$B$2:$B$10</definedName>
     <definedName name="_xlchart.v2.17" hidden="1">compareTreeTime!$C$1</definedName>
@@ -67,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="17">
   <si>
     <t>Input File</t>
   </si>
@@ -115,6 +115,9 @@
   </si>
   <si>
     <t>compareTreeTime (Codio)</t>
+  </si>
+  <si>
+    <t>equal</t>
   </si>
 </sst>
 </file>
@@ -250,7 +253,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>hashTime!$C$30</c:f>
+              <c:f>hashTime!$C$31</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -285,7 +288,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>(hashTime!$B$31:$B$35,hashTime!$B$37:$B$60,hashTime!$B$36)</c:f>
+              <c:f>(hashTime!$B$32:$B$36,hashTime!$B$38:$B$61,hashTime!$B$37)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="30"/>
@@ -384,7 +387,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>(hashTime!$C$31:$C$35,hashTime!$C$37:$C$60,hashTime!$C$60:$C$3631)</c:f>
+              <c:f>(hashTime!$C$32:$C$36,hashTime!$C$38:$C$61,hashTime!$C$61:$C$3632)</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="3601"/>
@@ -477,6 +480,9 @@
                 </c:pt>
                 <c:pt idx="29">
                   <c:v>3.5038E-2</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>3.5448E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -493,7 +499,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>hashTime!$D$30</c:f>
+              <c:f>hashTime!$D$31</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -528,7 +534,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>(hashTime!$B$31:$B$35,hashTime!$B$37:$B$60,hashTime!$B$36)</c:f>
+              <c:f>(hashTime!$B$32:$B$36,hashTime!$B$38:$B$61,hashTime!$B$37)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="30"/>
@@ -627,7 +633,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>(hashTime!$D$31:$D$35,hashTime!$D$37:$D$60,hashTime!$D$36)</c:f>
+              <c:f>(hashTime!$D$32:$D$36,hashTime!$D$38:$D$61,hashTime!$D$37)</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="30"/>
@@ -2035,7 +2041,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>hashTime!$B$31:$B$36</c:f>
+              <c:f>hashTime!$B$32:$B$37</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -2062,7 +2068,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>hashTime!$C$31:$C$36</c:f>
+              <c:f>hashTime!$C$32:$C$37</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="6"/>
@@ -2119,7 +2125,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>hashTime!$B$31:$B$36</c:f>
+              <c:f>hashTime!$B$32:$B$37</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -2146,7 +2152,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>hashTime!$D$31:$D$36</c:f>
+              <c:f>hashTime!$D$32:$D$37</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="6"/>
@@ -10800,13 +10806,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>12700</xdr:colOff>
-      <xdr:row>30</xdr:row>
+      <xdr:row>31</xdr:row>
       <xdr:rowOff>6350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>457200</xdr:colOff>
-      <xdr:row>43</xdr:row>
+      <xdr:row>44</xdr:row>
       <xdr:rowOff>107950</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -10872,13 +10878,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>12700</xdr:colOff>
-      <xdr:row>43</xdr:row>
+      <xdr:row>44</xdr:row>
       <xdr:rowOff>120650</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>457200</xdr:colOff>
-      <xdr:row>57</xdr:row>
+      <xdr:row>58</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -10914,7 +10920,7 @@
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>463550</xdr:colOff>
-      <xdr:row>28</xdr:row>
+      <xdr:row>29</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -11436,10 +11442,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4C55DF3-38C7-554C-AEC3-59F244130C35}">
-  <dimension ref="A1:D60"/>
+  <dimension ref="A1:D62"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H62" sqref="H62"/>
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="C62" sqref="C62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -11842,35 +11848,33 @@
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C29" s="1"/>
+      <c r="A29" t="s">
+        <v>3</v>
+      </c>
+      <c r="B29" t="s">
+        <v>16</v>
+      </c>
+      <c r="C29" s="1">
+        <v>1.4667E-3</v>
+      </c>
       <c r="D29" s="1"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
-        <v>0</v>
-      </c>
-      <c r="B30" t="s">
-        <v>1</v>
-      </c>
-      <c r="C30" t="s">
-        <v>5</v>
-      </c>
-      <c r="D30" t="s">
-        <v>6</v>
-      </c>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>4</v>
-      </c>
-      <c r="B31">
+        <v>0</v>
+      </c>
+      <c r="B31" t="s">
         <v>1</v>
       </c>
-      <c r="C31" s="1">
-        <v>1.9782000000000001E-2</v>
-      </c>
-      <c r="D31" s="1">
-        <v>5.0639000000000003E-2</v>
+      <c r="C31" t="s">
+        <v>5</v>
+      </c>
+      <c r="D31" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
@@ -11878,13 +11882,13 @@
         <v>4</v>
       </c>
       <c r="B32">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C32" s="1">
-        <v>1.9768999999999998E-2</v>
+        <v>1.9782000000000001E-2</v>
       </c>
       <c r="D32" s="1">
-        <v>3.6077999999999999E-2</v>
+        <v>5.0639000000000003E-2</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
@@ -11892,13 +11896,13 @@
         <v>4</v>
       </c>
       <c r="B33">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C33" s="1">
-        <v>2.2658999999999999E-2</v>
+        <v>1.9768999999999998E-2</v>
       </c>
       <c r="D33" s="1">
-        <v>3.9251000000000001E-2</v>
+        <v>3.6077999999999999E-2</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
@@ -11906,13 +11910,13 @@
         <v>4</v>
       </c>
       <c r="B34">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C34" s="1">
-        <v>2.8877E-2</v>
+        <v>2.2658999999999999E-2</v>
       </c>
       <c r="D34" s="1">
-        <v>3.1698999999999998E-2</v>
+        <v>3.9251000000000001E-2</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
@@ -11920,13 +11924,13 @@
         <v>4</v>
       </c>
       <c r="B35">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C35" s="1">
-        <v>3.2474999999999997E-2</v>
+        <v>2.8877E-2</v>
       </c>
       <c r="D35" s="1">
-        <v>3.4675999999999998E-2</v>
+        <v>3.1698999999999998E-2</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
@@ -11934,13 +11938,13 @@
         <v>4</v>
       </c>
       <c r="B36">
-        <v>100000</v>
+        <v>16</v>
       </c>
       <c r="C36" s="1">
-        <v>3.3197999999999998E-2</v>
+        <v>3.2474999999999997E-2</v>
       </c>
       <c r="D36" s="1">
-        <v>3.8855000000000001E-2</v>
+        <v>3.4675999999999998E-2</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
@@ -11948,13 +11952,13 @@
         <v>4</v>
       </c>
       <c r="B37">
-        <v>4000</v>
+        <v>100000</v>
       </c>
       <c r="C37" s="1">
-        <v>5.5432000000000002E-2</v>
+        <v>3.3197999999999998E-2</v>
       </c>
       <c r="D37" s="1">
-        <v>3.4883999999999998E-2</v>
+        <v>3.8855000000000001E-2</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
@@ -11962,13 +11966,13 @@
         <v>4</v>
       </c>
       <c r="B38">
-        <v>8000</v>
+        <v>4000</v>
       </c>
       <c r="C38" s="1">
-        <v>3.6507999999999999E-2</v>
+        <v>5.5432000000000002E-2</v>
       </c>
       <c r="D38" s="1">
-        <v>3.7811999999999998E-2</v>
+        <v>3.4883999999999998E-2</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
@@ -11976,13 +11980,13 @@
         <v>4</v>
       </c>
       <c r="B39">
-        <v>12000</v>
+        <v>8000</v>
       </c>
       <c r="C39" s="1">
-        <v>3.5895999999999997E-2</v>
+        <v>3.6507999999999999E-2</v>
       </c>
       <c r="D39" s="1">
-        <v>3.5541000000000003E-2</v>
+        <v>3.7811999999999998E-2</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
@@ -11990,13 +11994,13 @@
         <v>4</v>
       </c>
       <c r="B40">
-        <v>16000</v>
+        <v>12000</v>
       </c>
       <c r="C40" s="1">
-        <v>3.6112999999999999E-2</v>
+        <v>3.5895999999999997E-2</v>
       </c>
       <c r="D40" s="1">
-        <v>3.9115999999999998E-2</v>
+        <v>3.5541000000000003E-2</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
@@ -12004,13 +12008,13 @@
         <v>4</v>
       </c>
       <c r="B41">
-        <v>20000</v>
+        <v>16000</v>
       </c>
       <c r="C41" s="1">
-        <v>3.4486999999999997E-2</v>
+        <v>3.6112999999999999E-2</v>
       </c>
       <c r="D41" s="1">
-        <v>3.6905E-2</v>
+        <v>3.9115999999999998E-2</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
@@ -12018,13 +12022,13 @@
         <v>4</v>
       </c>
       <c r="B42">
-        <v>24000</v>
+        <v>20000</v>
       </c>
       <c r="C42" s="1">
-        <v>3.5027000000000003E-2</v>
+        <v>3.4486999999999997E-2</v>
       </c>
       <c r="D42" s="1">
-        <v>3.9047999999999999E-2</v>
+        <v>3.6905E-2</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
@@ -12032,13 +12036,13 @@
         <v>4</v>
       </c>
       <c r="B43">
-        <v>28000</v>
+        <v>24000</v>
       </c>
       <c r="C43" s="1">
-        <v>3.5749999999999997E-2</v>
+        <v>3.5027000000000003E-2</v>
       </c>
       <c r="D43" s="1">
-        <v>3.422E-2</v>
+        <v>3.9047999999999999E-2</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
@@ -12046,13 +12050,13 @@
         <v>4</v>
       </c>
       <c r="B44">
-        <v>32000</v>
+        <v>28000</v>
       </c>
       <c r="C44" s="1">
-        <v>3.4070000000000003E-2</v>
+        <v>3.5749999999999997E-2</v>
       </c>
       <c r="D44" s="1">
-        <v>3.8087999999999997E-2</v>
+        <v>3.422E-2</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
@@ -12060,13 +12064,13 @@
         <v>4</v>
       </c>
       <c r="B45">
-        <v>36000</v>
+        <v>32000</v>
       </c>
       <c r="C45" s="1">
-        <v>3.415E-2</v>
+        <v>3.4070000000000003E-2</v>
       </c>
       <c r="D45" s="1">
-        <v>3.8012999999999998E-2</v>
+        <v>3.8087999999999997E-2</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
@@ -12074,13 +12078,13 @@
         <v>4</v>
       </c>
       <c r="B46">
-        <v>40000</v>
+        <v>36000</v>
       </c>
       <c r="C46" s="1">
-        <v>3.4589000000000002E-2</v>
+        <v>3.415E-2</v>
       </c>
       <c r="D46" s="1">
-        <v>3.5187000000000003E-2</v>
+        <v>3.8012999999999998E-2</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
@@ -12088,13 +12092,13 @@
         <v>4</v>
       </c>
       <c r="B47">
-        <v>44000</v>
+        <v>40000</v>
       </c>
       <c r="C47" s="1">
-        <v>3.3218999999999999E-2</v>
+        <v>3.4589000000000002E-2</v>
       </c>
       <c r="D47" s="1">
-        <v>3.4916000000000003E-2</v>
+        <v>3.5187000000000003E-2</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
@@ -12102,13 +12106,13 @@
         <v>4</v>
       </c>
       <c r="B48">
-        <v>48000</v>
+        <v>44000</v>
       </c>
       <c r="C48" s="1">
-        <v>3.3729000000000002E-2</v>
+        <v>3.3218999999999999E-2</v>
       </c>
       <c r="D48" s="1">
-        <v>3.4422000000000001E-2</v>
+        <v>3.4916000000000003E-2</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
@@ -12116,13 +12120,13 @@
         <v>4</v>
       </c>
       <c r="B49">
-        <v>52000</v>
+        <v>48000</v>
       </c>
       <c r="C49" s="1">
-        <v>3.4872E-2</v>
+        <v>3.3729000000000002E-2</v>
       </c>
       <c r="D49" s="1">
-        <v>3.594E-2</v>
+        <v>3.4422000000000001E-2</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
@@ -12130,13 +12134,13 @@
         <v>4</v>
       </c>
       <c r="B50">
-        <v>56000</v>
+        <v>52000</v>
       </c>
       <c r="C50" s="1">
-        <v>3.381E-2</v>
+        <v>3.4872E-2</v>
       </c>
       <c r="D50" s="1">
-        <v>3.7282000000000003E-2</v>
+        <v>3.594E-2</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
@@ -12144,13 +12148,13 @@
         <v>4</v>
       </c>
       <c r="B51">
-        <v>60000</v>
+        <v>56000</v>
       </c>
       <c r="C51" s="1">
-        <v>3.4944999999999997E-2</v>
+        <v>3.381E-2</v>
       </c>
       <c r="D51" s="1">
-        <v>3.6230999999999999E-2</v>
+        <v>3.7282000000000003E-2</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
@@ -12158,13 +12162,13 @@
         <v>4</v>
       </c>
       <c r="B52">
-        <v>64000</v>
+        <v>60000</v>
       </c>
       <c r="C52" s="1">
-        <v>3.4113999999999998E-2</v>
+        <v>3.4944999999999997E-2</v>
       </c>
       <c r="D52" s="1">
-        <v>3.5249000000000003E-2</v>
+        <v>3.6230999999999999E-2</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
@@ -12172,13 +12176,13 @@
         <v>4</v>
       </c>
       <c r="B53">
-        <v>68000</v>
+        <v>64000</v>
       </c>
       <c r="C53" s="1">
-        <v>3.4902000000000002E-2</v>
+        <v>3.4113999999999998E-2</v>
       </c>
       <c r="D53" s="1">
-        <v>3.7032000000000002E-2</v>
+        <v>3.5249000000000003E-2</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
@@ -12186,13 +12190,13 @@
         <v>4</v>
       </c>
       <c r="B54">
-        <v>72000</v>
+        <v>68000</v>
       </c>
       <c r="C54" s="1">
-        <v>3.3154000000000003E-2</v>
+        <v>3.4902000000000002E-2</v>
       </c>
       <c r="D54" s="1">
-        <v>4.5338000000000003E-2</v>
+        <v>3.7032000000000002E-2</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
@@ -12200,13 +12204,13 @@
         <v>4</v>
       </c>
       <c r="B55">
-        <v>76000</v>
+        <v>72000</v>
       </c>
       <c r="C55" s="1">
-        <v>3.5445999999999998E-2</v>
+        <v>3.3154000000000003E-2</v>
       </c>
       <c r="D55" s="1">
-        <v>3.8406000000000003E-2</v>
+        <v>4.5338000000000003E-2</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
@@ -12214,13 +12218,13 @@
         <v>4</v>
       </c>
       <c r="B56">
-        <v>80000</v>
+        <v>76000</v>
       </c>
       <c r="C56" s="1">
-        <v>3.5421000000000001E-2</v>
+        <v>3.5445999999999998E-2</v>
       </c>
       <c r="D56" s="1">
-        <v>3.6540000000000003E-2</v>
+        <v>3.8406000000000003E-2</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
@@ -12228,13 +12232,13 @@
         <v>4</v>
       </c>
       <c r="B57">
-        <v>84000</v>
+        <v>80000</v>
       </c>
       <c r="C57" s="1">
-        <v>3.4957000000000002E-2</v>
+        <v>3.5421000000000001E-2</v>
       </c>
       <c r="D57" s="1">
-        <v>4.6136999999999997E-2</v>
+        <v>3.6540000000000003E-2</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
@@ -12242,13 +12246,13 @@
         <v>4</v>
       </c>
       <c r="B58">
-        <v>88000</v>
+        <v>84000</v>
       </c>
       <c r="C58" s="1">
-        <v>3.9886999999999999E-2</v>
+        <v>3.4957000000000002E-2</v>
       </c>
       <c r="D58" s="1">
-        <v>3.5991000000000002E-2</v>
+        <v>4.6136999999999997E-2</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
@@ -12256,13 +12260,13 @@
         <v>4</v>
       </c>
       <c r="B59">
-        <v>92000</v>
+        <v>88000</v>
       </c>
       <c r="C59" s="1">
-        <v>3.3066999999999999E-2</v>
+        <v>3.9886999999999999E-2</v>
       </c>
       <c r="D59" s="1">
-        <v>3.6503000000000001E-2</v>
+        <v>3.5991000000000002E-2</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
@@ -12270,13 +12274,38 @@
         <v>4</v>
       </c>
       <c r="B60">
+        <v>92000</v>
+      </c>
+      <c r="C60" s="1">
+        <v>3.3066999999999999E-2</v>
+      </c>
+      <c r="D60" s="1">
+        <v>3.6503000000000001E-2</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>4</v>
+      </c>
+      <c r="B61">
         <v>96000</v>
       </c>
-      <c r="C60" s="1">
+      <c r="C61" s="1">
         <v>3.5038E-2</v>
       </c>
-      <c r="D60" s="1">
+      <c r="D61" s="1">
         <v>3.5777999999999997E-2</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>4</v>
+      </c>
+      <c r="B62" t="s">
+        <v>16</v>
+      </c>
+      <c r="C62" s="1">
+        <v>3.5448E-2</v>
       </c>
     </row>
   </sheetData>
@@ -12289,8 +12318,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF848154-B09C-7541-99EC-D60136F45A46}">
   <dimension ref="A1:E55"/>
   <sheetViews>
-    <sheetView zoomScale="62" workbookViewId="0">
-      <selection activeCell="O43" sqref="O43"/>
+    <sheetView topLeftCell="A6" zoomScale="62" workbookViewId="0">
+      <selection activeCell="A36" sqref="A36:XFD36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -13059,7 +13088,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B36718F5-1030-AA4B-B6AA-4B2B10738B16}">
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
finish report and program
</commit_message>
<xml_diff>
--- a/simple-hashTimes.xlsx
+++ b/simple-hashTimes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/johnpeterson/Documents/UTexas CS/PS/cs380p-f23/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEE56CA5-F3C9-0945-8820-A54BA5713466}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72C80F08-654A-0E4D-ACFD-E04391AC0426}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2380" yWindow="3500" windowWidth="31980" windowHeight="17440" activeTab="2" xr2:uid="{09B1B139-03D2-1C4D-B9A6-5AC75A022D8A}"/>
   </bookViews>
@@ -13102,8 +13102,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B36718F5-1030-AA4B-B6AA-4B2B10738B16}">
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C11"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="200" workbookViewId="0">
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>